<commit_message>
Restructured project and added more OCR implementation flavors.
</commit_message>
<xml_diff>
--- a/work/output.xlsx
+++ b/work/output.xlsx
@@ -1,122 +1,121 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/thomas_endt_uipath_com/Documents/Documents/UiPath/MailToSap_Steffen/work/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_0859E3757107AE2F867E1E5BB3A546D127D41131" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{8E888A21-8C4A-47EB-B594-0D9D4AF36D00}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <x:sheet name="Simple Fields" sheetId="5" r:id="rId5"/>
-    <x:sheet name="Simple Fields - Formatted" sheetId="6" r:id="rId6"/>
-    <x:sheet name="LineItems" sheetId="7" r:id="rId7"/>
-    <x:sheet name="LineItems - Formatted" sheetId="8" r:id="rId8"/>
+    <x:sheet name="Simple Fields" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Simple Fields - Formatted" sheetId="5" r:id="rId5"/>
+    <x:sheet name="Items" sheetId="7" r:id="rId7"/>
+    <x:sheet name="Items - Formatted" sheetId="8" r:id="rId8"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="0"/>
+  <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <x:si>
+    <x:t>Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor-addr</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Billing-addr</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shipping-addr</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Invoice-no</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Po-no</x:t>
+  </x:si>
   <x:si>
     <x:t>Date</x:t>
   </x:si>
   <x:si>
-    <x:t>Due Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Invoice#</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Customer ID</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Supplier</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Subtotal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tax Rate</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tax Due</x:t>
-  </x:si>
-  <x:si>
     <x:t>Total</x:t>
   </x:si>
   <x:si>
-    <x:t>LineItems</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4/7/2019</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5/22/2019</x:t>
+    <x:t>Tax</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Currency</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Items</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tiefland Glass AG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>123 Basedow Street Leipzig,DE,04277</x:t>
+  </x:si>
+  <x:si>
+    <x:t>231 Lyoner Street Frankfurt,DE,60441</x:t>
   </x:si>
   <x:si>
     <x:t>850888</x:t>
   </x:si>
   <x:si>
-    <x:t>A700</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tiefland Glass AG</x:t>
+    <x:t>2019-04-07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5500.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>500.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EUR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>table</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Description</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Unit-price</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Quantity</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Line-amount</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Item-po-no</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Professional services</x:t>
   </x:si>
   <x:si>
     <x:t>5,000.00</x:t>
   </x:si>
   <x:si>
-    <x:t>500.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5,500.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>table</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Description</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Unit Price</x:t>
-  </x:si>
-  <x:si>
-    <x:t>QTY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Taxed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Amount</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Professional services</x:t>
-  </x:si>
-  <x:si>
     <x:t>1</x:t>
   </x:si>
   <x:si>
-    <x:t>X</x:t>
+    <x:t>5000.00</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1" x14ac:knownFonts="1">
+  <x:fonts count="1">
     <x:font>
+      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -132,23 +131,30 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+  <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="3">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  <x:cellXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -157,19 +163,10 @@
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
 </x:styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -452,29 +449,81 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G1"/>
+  <x:dimension ref="A1:K2"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A1" sqref="A1 A1:A1 A1:P6"/>
-    </x:sheetView>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <x:cols>
-    <x:col min="1" max="1" width="11.199219" style="2" customWidth="1"/>
-    <x:col min="2" max="2" width="12.464844" style="2" customWidth="1"/>
-    <x:col min="3" max="3" width="11.464844" style="2" customWidth="1"/>
-    <x:col min="4" max="4" width="9.132812" style="2" customWidth="1"/>
-    <x:col min="5" max="5" width="11.464844" style="2" customWidth="1"/>
-    <x:col min="6" max="6" width="29.132812" style="2" customWidth="1"/>
-    <x:col min="7" max="7" width="19.132812" style="2" customWidth="1"/>
-  </x:cols>
+  <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:7"/>
+    <x:row r="1" spans="1:11">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:11">
+      <x:c r="A2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K2" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
@@ -489,71 +538,74 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G2"/>
+  <x:dimension ref="A1:K2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:10">
-      <x:c r="A1" s="2" t="s">
+    <x:row r="1" spans="1:11">
+      <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="2" t="s">
+      <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="2" t="s">
+      <x:c r="C1" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="2" t="s">
+      <x:c r="D1" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="2" t="s">
+      <x:c r="E1" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="2" t="s">
+      <x:c r="F1" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G1" s="2" t="s">
+      <x:c r="G1" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H1" s="2" t="s">
+      <x:c r="H1" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="I1" s="2" t="s">
+      <x:c r="I1" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="J1" s="2" t="s">
+      <x:c r="J1" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
+      <x:c r="K1" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:10">
-      <x:c r="A2" s="2" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B2" s="2" t="s">
+    <x:row r="2" spans="1:11">
+      <x:c r="A2" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="C2" s="2" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D2" s="2" t="s">
+      <x:c r="C2" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="E2" s="2" t="s">
+      <x:c r="E2" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="F2" s="2" t="s">
+      <x:c r="G2" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="H2" s="2" t="s">
+      <x:c r="H2" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="I2" s="2" t="s">
+      <x:c r="I2" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="J2" s="2" t="s">
+      <x:c r="J2" s="0" t="s">
         <x:v>18</x:v>
+      </x:c>
+      <x:c r="K2" s="0" t="s">
+        <x:v>19</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -570,71 +622,41 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G2"/>
+  <x:dimension ref="A1:E2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:10">
-      <x:c r="A1" s="2" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="2" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D1" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E1" s="2" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="F1" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="G1" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="H1" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="I1" s="2" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="J1" s="2" t="s">
-        <x:v>9</x:v>
+    <x:row r="1" spans="1:5">
+      <x:c r="A1" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>24</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:10">
-      <x:c r="A2" s="2" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B2" s="2" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C2" s="2" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="D2" s="2" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="E2" s="2" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="F2" s="2" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="H2" s="2" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="I2" s="2" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="J2" s="2" t="s">
-        <x:v>18</x:v>
+    <x:row r="2" spans="1:5">
+      <x:c r="A2" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>28</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -658,91 +680,34 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
     <x:row r="1" spans="1:5">
-      <x:c r="A1" s="2" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="B1" s="2" t="s">
+      <x:c r="A1" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="C1" s="2" t="s">
+      <x:c r="B1" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="D1" s="2" t="s">
+      <x:c r="C1" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="E1" s="2" t="s">
+      <x:c r="D1" s="0" t="s">
         <x:v>23</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5">
-      <x:c r="A2" s="2" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="B2" s="2" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C2" s="2" t="s">
+      <x:c r="A2" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="D2" s="2" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="E2" s="2" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:E2"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:5">
-      <x:c r="A1" s="2" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="B1" s="2" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="C1" s="2" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="D1" s="2" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="E1" s="2" t="s">
-        <x:v>23</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:5">
-      <x:c r="A2" s="2" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="B2" s="2" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C2" s="2" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="D2" s="2" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="E2" s="2" t="s">
-        <x:v>15</x:v>
+      <x:c r="C2" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>28</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Version before adding human in the loop invoice approval
</commit_message>
<xml_diff>
--- a/work/output.xlsx
+++ b/work/output.xlsx
@@ -10,6 +10,8 @@
     <x:sheet name="Simple Fields - Formatted" sheetId="5" r:id="rId5"/>
     <x:sheet name="Items" sheetId="7" r:id="rId7"/>
     <x:sheet name="Items - Formatted" sheetId="8" r:id="rId8"/>
+    <x:sheet name="LineItems" sheetId="9" r:id="rId9"/>
+    <x:sheet name="LineItems - Formatted" sheetId="10" r:id="rId10"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -17,66 +19,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
-  <x:si>
-    <x:t>Name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vendor-addr</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Billing-addr</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Shipping-addr</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Invoice-no</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Po-no</x:t>
-  </x:si>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <x:si>
     <x:t>Date</x:t>
   </x:si>
   <x:si>
+    <x:t>Due Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Invoice#</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Customer ID</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Supplier</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Subtotal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tax Rate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tax Due</x:t>
+  </x:si>
+  <x:si>
     <x:t>Total</x:t>
   </x:si>
   <x:si>
-    <x:t>Tax</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Currency</x:t>
+    <x:t>LineItems</x:t>
   </x:si>
   <x:si>
     <x:t>Items</x:t>
   </x:si>
   <x:si>
+    <x:t>4/7/2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5/22/2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>850888</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A700</x:t>
+  </x:si>
+  <x:si>
     <x:t>Tiefland Glass AG</x:t>
   </x:si>
   <x:si>
-    <x:t>123 Basedow Street Leipzig,DE,04277</x:t>
-  </x:si>
-  <x:si>
-    <x:t>231 Lyoner Street Frankfurt,DE,60441</x:t>
-  </x:si>
-  <x:si>
-    <x:t>850888</x:t>
+    <x:t>5,000.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>500.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5,500.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>table</x:t>
   </x:si>
   <x:si>
     <x:t>2019-04-07</x:t>
   </x:si>
   <x:si>
-    <x:t>5500.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>500.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EUR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>table</x:t>
+    <x:t>2019-05-22</x:t>
   </x:si>
   <x:si>
     <x:t>Description</x:t>
@@ -97,13 +105,25 @@
     <x:t>Professional services</x:t>
   </x:si>
   <x:si>
-    <x:t>5,000.00</x:t>
-  </x:si>
-  <x:si>
     <x:t>1</x:t>
   </x:si>
   <x:si>
     <x:t>5000.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Unit Price</x:t>
+  </x:si>
+  <x:si>
+    <x:t>QTY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Taxed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Amount</x:t>
+  </x:si>
+  <x:si>
+    <x:t>X</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -505,20 +525,23 @@
       <x:c r="C2" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
       <x:c r="H2" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="I2" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="J2" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="K2" s="0" t="s">
         <x:v>19</x:v>
@@ -581,28 +604,31 @@
     </x:row>
     <x:row r="2" spans="1:11">
       <x:c r="A2" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
       <x:c r="H2" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="I2" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="J2" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="K2" s="0" t="s">
         <x:v>19</x:v>
@@ -630,33 +656,33 @@
   <x:sheetData>
     <x:row r="1" spans="1:5">
       <x:c r="A1" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="E1" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5">
       <x:c r="A2" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -681,33 +707,141 @@
   <x:sheetData>
     <x:row r="1" spans="1:5">
       <x:c r="A1" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="E1" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5">
       <x:c r="A2" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:E2"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:5">
+      <x:c r="A1" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5">
+      <x:c r="A2" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
       <x:c r="D2" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:E2"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:5">
+      <x:c r="A1" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5">
+      <x:c r="A2" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
         <x:v>28</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>16</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>